<commit_message>
Normalize line endings to LF
</commit_message>
<xml_diff>
--- a/testfiles/policy.xlsx
+++ b/testfiles/policy.xlsx
@@ -29,7 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>生效日期</t>
+    <t>编号</t>
   </si>
   <si>
     <t>总净重(KG)</t>
@@ -87,7 +87,7 @@
     <t>汇率(RMB/美元)</t>
   </si>
   <si>
-    <t>2025.4.1</t>
+    <t>001</t>
   </si>
 </sst>
 </file>
@@ -750,6 +750,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1099,7 +1100,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83636363636364" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="7"/>
@@ -1140,7 +1141,7 @@
       </c>
     </row>
     <row r="2" ht="14.5" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">

</xml_diff>